<commit_message>
added class_time field to card model
</commit_message>
<xml_diff>
--- a/backend/app/mod_gate/static/卡片上传模版.xlsx
+++ b/backend/app/mod_gate/static/卡片上传模版.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desmond/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desmond/Repos/quatek_web_app_project/backend/app/mod_gate/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F234401D-0C5A-1F4D-8EC3-4ECD2D87DC04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8641BA05-3BDE-1E4F-88CD-B5E386C06829}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="1540" windowWidth="28240" windowHeight="17440" xr2:uid="{8E4751AF-3E20-AD4B-B372-A0715642368F}"/>
+    <workbookView xWindow="4100" yWindow="460" windowWidth="28240" windowHeight="17440" xr2:uid="{8E4751AF-3E20-AD4B-B372-A0715642368F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>*card_number</t>
   </si>
@@ -67,7 +67,12 @@
     <t>*gender(0:female|1:male)</t>
   </si>
   <si>
+    <t>班别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -435,9 +440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE6C2F9-991B-FB42-BBF4-B6731E9B1ED6}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -450,7 +457,7 @@
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,6 +477,9 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added multi classes support
</commit_message>
<xml_diff>
--- a/backend/app/mod_gate/static/卡片上传模版.xlsx
+++ b/backend/app/mod_gate/static/卡片上传模版.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desmond/Repos/quatek_web_app_project/backend/app/mod_gate/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8641BA05-3BDE-1E4F-88CD-B5E386C06829}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23941E6A-68B9-F848-A5E2-53EE4ED5E5F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="460" windowWidth="28240" windowHeight="17440" xr2:uid="{8E4751AF-3E20-AD4B-B372-A0715642368F}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="28240" windowHeight="17440" xr2:uid="{8E4751AF-3E20-AD4B-B372-A0715642368F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,11 +67,11 @@
     <t>*gender(0:female|1:male)</t>
   </si>
   <si>
-    <t>班别</t>
+    <t>note</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>note</t>
+    <t>classes (class1,class2,class3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -443,7 +443,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -477,10 +477,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed card number normalizing bugs in routers.py
</commit_message>
<xml_diff>
--- a/backend/app/mod_gate/static/卡片上传模版.xlsx
+++ b/backend/app/mod_gate/static/卡片上传模版.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desmond/Repos/quatek_web_app_project/backend/app/mod_gate/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23941E6A-68B9-F848-A5E2-53EE4ED5E5F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354C3596-4C79-6144-AD2D-F3E5C16C0169}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28240" windowHeight="17440" xr2:uid="{8E4751AF-3E20-AD4B-B372-A0715642368F}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>*card_number</t>
   </si>
@@ -72,6 +72,10 @@
   </si>
   <si>
     <t>classes (class1,class2,class3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HID card number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -440,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE6C2F9-991B-FB42-BBF4-B6731E9B1ED6}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -457,7 +461,7 @@
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,6 +485,9 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>